<commit_message>
back to original models
</commit_message>
<xml_diff>
--- a/DTDL Models/cheese-factory-scenario.xlsx
+++ b/DTDL Models/cheese-factory-scenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\AzureDigitalTwinAz220Demo\CheeseCaveDevice\DTDL Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FFAF2F-CFD0-4FF8-A911-1DBE10003230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956F80EA-6FE0-4ABA-AF24-3EC685A4258F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{B6154E4F-774F-4730-84F3-5195ADBCD94E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>ModelID</t>
   </si>
@@ -100,9 +100,6 @@
     <t>rel_has_devices</t>
   </si>
   <si>
-    <t>{"desiredTemperature": 50, "desiredHumidity": 85, "temperature": 70, "humidity": 85, "inUse": true, "temperatureAlert": true, "humidityAlert": false, "fanAlert": true}</t>
-  </si>
-  <si>
     <t>dtmi:com:contoso:digital_factory:cheese_factory:cheese_cave;1</t>
   </si>
   <si>
@@ -118,16 +115,10 @@
     <t>cave_3</t>
   </si>
   <si>
-    <t>{"desiredTemperature": 50, "desiredHumidity": 85, "temperatureAlert": true, "humidityAlert": false, "fanAlert": true, "humidity":100, "temperature":42}</t>
-  </si>
-  <si>
-    <t>{"desiredTemperature": 50, "desiredHumidity": 85, "temperatureAlert": false, "humidityAlert": false, "fanAlert": false, "humidity":100, "temperature":42}</t>
-  </si>
-  <si>
-    <t>{"desiredTemperature": 50, "desiredHumidity": 85, "temperatureAlert": false, "humidityAlert": false, "fanAlert": false , "humidity":100, "temperature":42}</t>
-  </si>
-  <si>
-    <t>dtmi:com:contoso:digital_factory:cheese_factory:cheese_cave_device;2</t>
+    <t>dtmi:com:contoso:digital_factory:cheese_factory:cheese_cave_device;1</t>
+  </si>
+  <si>
+    <t>{"desiredTemperature": 50, "desiredHumidity": 85, "temperatureAlert": true, "humidityAlert": true, "fanAlert": true}</t>
   </si>
 </sst>
 </file>
@@ -488,7 +479,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -530,16 +521,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -547,16 +538,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -564,64 +555,64 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>

</xml_diff>